<commit_message>
Ajustar elementos en una hoja
</commit_message>
<xml_diff>
--- a/Excel/Práctica/5. Impresión en Excel/Cabecero y pie de pagina en Excel, ajustar elementos en una hoja, impresión de títulos.xlsx
+++ b/Excel/Práctica/5. Impresión en Excel/Cabecero y pie de pagina en Excel, ajustar elementos en una hoja, impresión de títulos.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="283">
   <si>
     <t>ID</t>
   </si>
@@ -1003,6 +1003,169 @@
   <si>
     <t>Por último podemos decidir si queremos que la primera página sea diferente a las demás o, bien, decidir si queremos diferenciar el diseño de las páginas pares del diseño de las páginas impares.</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">En el ejercicio de dar diseño de impresión en Excel, como lo estamos haciendo ahora, usted puede asistirse de una correcta configuración de la </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>orientación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de sus páginas para aprovechar al máximo los espacios de ellas; como por ejemplo, en los casos en los que requiere hacer uso de una orientación </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>horizontal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cuando precisa de más espacio a lo ancho de dichas páginas (como lo es este caso). Si se fija, al configurar este Excel con diseño de impresión en esta hoja de cálculo, ahora las columnas caben a lo ancho de sus páginas (anteriormente no). Sin embargo sepa que a la final todo depende de sus propias necesidades, en otras ocasiones quizas sería mejor optar por una orientación </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>vertical</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sin embargo, existe una manera más eficiente y precisa de hacer </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">caber </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">nuestro contenido, cualquiera que deseemos, dentro de una misma página de Excel al darle diseño de impresión a una hoja de cálculo en cuestión. ¿Nota las líneas azules de trazo intermitente situadas sobre esta misma hoja de cálculo, las que se ven con un diseño </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>normal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>? Esas son, justamente, las encargadas de delimitar los cortes de información a la hora de separar una página de otra.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve"> Así se ajustaría de manera efectiva los elementos dentro de una misma página al darle a la hoja de Excel un diseño de impresión. A este proceso se le llama: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">Escalamiento </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">y también se puede configurar manualmente en la opción </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">Configurar página </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">de la pestaña </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>Diseño de página.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1011,7 +1174,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -1093,6 +1256,24 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1163,7 +1344,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1173,6 +1354,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1860,10 +2044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P193"/>
+  <dimension ref="A1:P194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1925,16 +2109,16 @@
       <c r="G2" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1958,14 +2142,14 @@
       <c r="G3" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
     </row>
     <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -1989,14 +2173,14 @@
       <c r="G4" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
     </row>
     <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -2020,14 +2204,14 @@
       <c r="G5" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
     </row>
     <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -2051,14 +2235,14 @@
       <c r="G6" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
     </row>
     <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -2079,14 +2263,14 @@
       <c r="G7" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
     </row>
     <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -2110,14 +2294,14 @@
       <c r="G8" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
     </row>
     <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -2141,14 +2325,14 @@
       <c r="G9" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
     </row>
     <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -2172,14 +2356,14 @@
       <c r="G10" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
     </row>
     <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -2203,14 +2387,14 @@
       <c r="G11" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -2234,14 +2418,14 @@
       <c r="G12" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
     </row>
     <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -2265,14 +2449,14 @@
       <c r="G13" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
     </row>
     <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -2296,14 +2480,14 @@
       <c r="G14" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
     </row>
     <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -2327,14 +2511,14 @@
       <c r="G15" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
     </row>
     <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -2358,14 +2542,14 @@
       <c r="G16" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
     </row>
     <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -2389,14 +2573,14 @@
       <c r="G17" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
     </row>
     <row r="18" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -2420,14 +2604,14 @@
       <c r="G18" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
     </row>
     <row r="19" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -2471,12 +2655,12 @@
       <c r="G20" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
     </row>
     <row r="21" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -2615,16 +2799,16 @@
       <c r="G26" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="I26" s="9" t="s">
+      <c r="I26" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
     </row>
     <row r="27" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
@@ -2648,14 +2832,14 @@
       <c r="G27" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
     </row>
     <row r="28" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -2679,14 +2863,14 @@
       <c r="G28" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
     </row>
     <row r="29" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -2710,14 +2894,14 @@
       <c r="G29" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
     </row>
     <row r="30" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -2764,18 +2948,18 @@
       <c r="G31" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-    </row>
-    <row r="32" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+    </row>
+    <row r="32" spans="1:16" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>33</v>
       </c>
@@ -2797,16 +2981,16 @@
       <c r="G32" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-    </row>
-    <row r="33" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+    </row>
+    <row r="33" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>34</v>
       </c>
@@ -2828,8 +3012,16 @@
       <c r="G33" s="1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+    </row>
+    <row r="34" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>35</v>
       </c>
@@ -2852,7 +3044,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>36</v>
       </c>
@@ -2874,8 +3066,18 @@
       <c r="G35" s="1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+    </row>
+    <row r="36" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>37</v>
       </c>
@@ -2897,8 +3099,16 @@
       <c r="G36" s="1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+    </row>
+    <row r="37" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>38</v>
       </c>
@@ -2920,8 +3130,16 @@
       <c r="G37" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+    </row>
+    <row r="38" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>39</v>
       </c>
@@ -2943,8 +3161,16 @@
       <c r="G38" s="1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+    </row>
+    <row r="39" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>40</v>
       </c>
@@ -2966,8 +3192,16 @@
       <c r="G39" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+    </row>
+    <row r="40" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>41</v>
       </c>
@@ -2989,8 +3223,16 @@
       <c r="G40" s="5" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+    </row>
+    <row r="41" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>42</v>
       </c>
@@ -3012,8 +3254,16 @@
       <c r="G41" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+    </row>
+    <row r="42" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43</v>
       </c>
@@ -3036,7 +3286,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44</v>
       </c>
@@ -3058,8 +3308,18 @@
       <c r="G43" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I43" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+    </row>
+    <row r="44" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45</v>
       </c>
@@ -3081,8 +3341,16 @@
       <c r="G44" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+    </row>
+    <row r="45" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>46</v>
       </c>
@@ -3104,8 +3372,16 @@
       <c r="G45" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+    </row>
+    <row r="46" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>47</v>
       </c>
@@ -3127,8 +3403,16 @@
       <c r="G46" s="5" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="10"/>
+    </row>
+    <row r="47" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>48</v>
       </c>
@@ -3150,8 +3434,16 @@
       <c r="G47" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+    </row>
+    <row r="48" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>49</v>
       </c>
@@ -3173,8 +3465,16 @@
       <c r="G48" s="5" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+      <c r="N48" s="10"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+    </row>
+    <row r="49" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>50</v>
       </c>
@@ -3196,8 +3496,16 @@
       <c r="G49" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+      <c r="N49" s="10"/>
+      <c r="O49" s="10"/>
+      <c r="P49" s="10"/>
+    </row>
+    <row r="50" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>51</v>
       </c>
@@ -3219,8 +3527,16 @@
       <c r="G50" s="5" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+    </row>
+    <row r="51" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>52</v>
       </c>
@@ -3243,7 +3559,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>53</v>
       </c>
@@ -3266,7 +3582,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>54</v>
       </c>
@@ -3289,7 +3605,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>55</v>
       </c>
@@ -3312,7 +3628,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>56</v>
       </c>
@@ -3335,7 +3651,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>57</v>
       </c>
@@ -3358,7 +3674,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>58</v>
       </c>
@@ -3381,7 +3697,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>59</v>
       </c>
@@ -3404,7 +3720,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>60</v>
       </c>
@@ -3427,7 +3743,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>61</v>
       </c>
@@ -3450,7 +3766,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>62</v>
       </c>
@@ -3473,7 +3789,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>63</v>
       </c>
@@ -3496,7 +3812,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>64</v>
       </c>
@@ -3519,7 +3835,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>65</v>
       </c>
@@ -6480,7 +6796,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="193" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>200</v>
       </c>
@@ -6502,26 +6818,41 @@
       <c r="G193" s="5" t="s">
         <v>275</v>
       </c>
+    </row>
+    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I194" s="1"/>
+      <c r="J194" s="1"/>
+      <c r="K194" s="1"/>
+      <c r="L194" s="1"/>
+      <c r="M194" s="1"/>
+      <c r="N194" s="1"/>
+      <c r="O194" s="1"/>
+      <c r="P194" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:G193">
     <sortCondition ref="A2"/>
   </sortState>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="I43:P50"/>
+    <mergeCell ref="I35:P41"/>
+    <mergeCell ref="I31:P32"/>
     <mergeCell ref="I2:P18"/>
     <mergeCell ref="I20:L20"/>
     <mergeCell ref="I26:P29"/>
-    <mergeCell ref="I31:P32"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="77" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;F&amp;R&amp;P</oddHeader>
     <oddFooter>&amp;C&amp;P de &amp;N</oddFooter>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="33" max="16383" man="1"/>
+  </rowBreaks>
   <colBreaks count="2" manualBreakCount="2">
-    <brk id="10" max="1048575" man="1"/>
+    <brk id="8" max="1048575" man="1"/>
     <brk id="31" max="1048575" man="1"/>
   </colBreaks>
   <drawing r:id="rId2"/>

</xml_diff>